<commit_message>
4 cases done with screenshots and documentation
</commit_message>
<xml_diff>
--- a/Files/simple.xlsx
+++ b/Files/simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python-appium\simple-demo\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BF494C-5C19-48CE-84CC-6C49E01B9B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FC3E69-F574-4ABE-B219-3AF0DE1F4242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>TC1</t>
   </si>
@@ -79,6 +79,51 @@
   </si>
   <si>
     <t>13. Click Skip</t>
+  </si>
+  <si>
+    <t>1. Click the patient search box (Enter name, phone or ID)</t>
+  </si>
+  <si>
+    <t>2. Click REGISTER AS A NEW PATIENT button</t>
+  </si>
+  <si>
+    <t>3. Fillout all the fields</t>
+  </si>
+  <si>
+    <t>4. Click Next button</t>
+  </si>
+  <si>
+    <t>5. Select NO for all disease</t>
+  </si>
+  <si>
+    <t>6. Select YES for all disease</t>
+  </si>
+  <si>
+    <t>7. Click save</t>
+  </si>
+  <si>
+    <t>8. Click Not Now</t>
+  </si>
+  <si>
+    <t>9. Validate patient if exist via search</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>1. Click Medicine (+) button</t>
+  </si>
+  <si>
+    <t>2. Select multiple kinds of existing medicines and their dosage</t>
+  </si>
+  <si>
+    <t>3. Click Save</t>
+  </si>
+  <si>
+    <t>4. Validate if the selected medicines reflected in the medicine section</t>
+  </si>
+  <si>
+    <t>TC5</t>
   </si>
 </sst>
 </file>
@@ -403,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,6 +546,81 @@
         <v>2</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>